<commit_message>
fixed error in data
</commit_message>
<xml_diff>
--- a/data/influenza.xlsx
+++ b/data/influenza.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/27d0b5489d3113a0/Common Files/BootcampShare/Projects/ai-bootcamp-project-1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="466" documentId="8_{6F5A5966-C440-4252-8159-6308A6958721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDDD978B-5B66-4EB4-8F16-862AF5B749F1}"/>
+  <xr:revisionPtr revIDLastSave="469" documentId="8_{6F5A5966-C440-4252-8159-6308A6958721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2F1378B-FB18-48E9-8027-54DCFA1BA8F7}"/>
   <bookViews>
-    <workbookView xWindow="25035" yWindow="2850" windowWidth="20835" windowHeight="15645" xr2:uid="{7213F9FE-3F13-4400-A951-9EE5221AE410}"/>
+    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="10524" xr2:uid="{7213F9FE-3F13-4400-A951-9EE5221AE410}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -119,6 +119,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,16 +444,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C442379A-3B83-4E79-ADD5-8F64604E3F7E}">
   <dimension ref="A1:J191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="C159" sqref="C159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="3" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -481,7 +485,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>2017</v>
       </c>
@@ -516,7 +520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2017</v>
       </c>
@@ -551,7 +555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>2017</v>
       </c>
@@ -588,7 +592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>2017</v>
       </c>
@@ -625,7 +629,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>2017</v>
       </c>
@@ -662,7 +666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>2017</v>
       </c>
@@ -699,7 +703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>2017</v>
       </c>
@@ -736,7 +740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>2017</v>
       </c>
@@ -773,7 +777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>2017</v>
       </c>
@@ -810,7 +814,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>2017</v>
       </c>
@@ -847,7 +851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>2017</v>
       </c>
@@ -884,7 +888,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>2017</v>
       </c>
@@ -921,7 +925,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>2017</v>
       </c>
@@ -958,7 +962,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -995,7 +999,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>2018</v>
       </c>
@@ -1032,7 +1036,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>2018</v>
       </c>
@@ -1069,7 +1073,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>2018</v>
       </c>
@@ -1106,7 +1110,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>2018</v>
       </c>
@@ -1143,7 +1147,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>2018</v>
       </c>
@@ -1180,7 +1184,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>2018</v>
       </c>
@@ -1217,7 +1221,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>2018</v>
       </c>
@@ -1254,7 +1258,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>2018</v>
       </c>
@@ -1291,7 +1295,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>2018</v>
       </c>
@@ -1328,7 +1332,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>2018</v>
       </c>
@@ -1365,7 +1369,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>2018</v>
       </c>
@@ -1402,7 +1406,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>2018</v>
       </c>
@@ -1439,7 +1443,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>2018</v>
       </c>
@@ -1476,7 +1480,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>2018</v>
       </c>
@@ -1513,7 +1517,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>2018</v>
       </c>
@@ -1550,7 +1554,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>2018</v>
       </c>
@@ -1587,7 +1591,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>2018</v>
       </c>
@@ -1624,7 +1628,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>2018</v>
       </c>
@@ -1661,7 +1665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>2018</v>
       </c>
@@ -1698,7 +1702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>2018</v>
       </c>
@@ -1723,7 +1727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>2018</v>
       </c>
@@ -1748,7 +1752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>2018</v>
       </c>
@@ -1773,7 +1777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <v>2018</v>
       </c>
@@ -1798,7 +1802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <v>2018</v>
       </c>
@@ -1823,7 +1827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>2018</v>
       </c>
@@ -1848,7 +1852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>2018</v>
       </c>
@@ -1873,7 +1877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>2018</v>
       </c>
@@ -1898,7 +1902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <v>2018</v>
       </c>
@@ -1923,7 +1927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <v>2018</v>
       </c>
@@ -1948,7 +1952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <v>2018</v>
       </c>
@@ -1973,7 +1977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <v>2018</v>
       </c>
@@ -1998,7 +2002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
         <v>2018</v>
       </c>
@@ -2023,7 +2027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <v>2018</v>
       </c>
@@ -2048,7 +2052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
         <v>2018</v>
       </c>
@@ -2073,7 +2077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <v>2018</v>
       </c>
@@ -2098,7 +2102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
         <v>2018</v>
       </c>
@@ -2123,7 +2127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
         <v>2018</v>
       </c>
@@ -2148,7 +2152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
         <v>2018</v>
       </c>
@@ -2173,7 +2177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
         <v>2018</v>
       </c>
@@ -2208,7 +2212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
         <v>2018</v>
       </c>
@@ -2245,7 +2249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
         <v>2018</v>
       </c>
@@ -2282,7 +2286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
         <v>2018</v>
       </c>
@@ -2319,7 +2323,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
         <v>2018</v>
       </c>
@@ -2356,7 +2360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A59">
         <v>2018</v>
       </c>
@@ -2393,7 +2397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A60">
         <v>2018</v>
       </c>
@@ -2430,7 +2434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A61">
         <v>2018</v>
       </c>
@@ -2467,7 +2471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
         <v>2018</v>
       </c>
@@ -2504,7 +2508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A63">
         <v>2018</v>
       </c>
@@ -2541,7 +2545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
         <v>2018</v>
       </c>
@@ -2578,7 +2582,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A65">
         <v>2018</v>
       </c>
@@ -2615,7 +2619,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A66">
         <v>2018</v>
       </c>
@@ -2652,7 +2656,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A67">
         <v>2019</v>
       </c>
@@ -2689,7 +2693,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A68">
         <v>2019</v>
       </c>
@@ -2726,7 +2730,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A69">
         <v>2019</v>
       </c>
@@ -2763,7 +2767,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A70">
         <v>2019</v>
       </c>
@@ -2800,7 +2804,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A71">
         <v>2019</v>
       </c>
@@ -2837,7 +2841,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A72">
         <v>2019</v>
       </c>
@@ -2874,7 +2878,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A73">
         <v>2019</v>
       </c>
@@ -2911,7 +2915,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A74">
         <v>2019</v>
       </c>
@@ -2948,7 +2952,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A75">
         <v>2019</v>
       </c>
@@ -2985,7 +2989,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A76">
         <v>2019</v>
       </c>
@@ -3022,7 +3026,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A77">
         <v>2019</v>
       </c>
@@ -3059,7 +3063,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A78">
         <v>2019</v>
       </c>
@@ -3096,7 +3100,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A79">
         <v>2019</v>
       </c>
@@ -3133,7 +3137,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A80">
         <v>2019</v>
       </c>
@@ -3170,7 +3174,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A81">
         <v>2019</v>
       </c>
@@ -3207,7 +3211,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A82">
         <v>2019</v>
       </c>
@@ -3244,7 +3248,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A83">
         <v>2019</v>
       </c>
@@ -3281,7 +3285,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A84">
         <v>2019</v>
       </c>
@@ -3318,7 +3322,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A85">
         <v>2019</v>
       </c>
@@ -3355,7 +3359,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A86">
         <v>2019</v>
       </c>
@@ -3392,7 +3396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A87">
         <v>2019</v>
       </c>
@@ -3417,7 +3421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A88">
         <v>2019</v>
       </c>
@@ -3442,7 +3446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A89">
         <v>2019</v>
       </c>
@@ -3467,7 +3471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A90">
         <v>2019</v>
       </c>
@@ -3492,7 +3496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A91">
         <v>2019</v>
       </c>
@@ -3517,7 +3521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A92">
         <v>2019</v>
       </c>
@@ -3542,7 +3546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A93">
         <v>2019</v>
       </c>
@@ -3567,7 +3571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A94">
         <v>2019</v>
       </c>
@@ -3592,7 +3596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A95">
         <v>2019</v>
       </c>
@@ -3617,7 +3621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A96">
         <v>2019</v>
       </c>
@@ -3642,7 +3646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A97">
         <v>2019</v>
       </c>
@@ -3667,7 +3671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A98">
         <v>2019</v>
       </c>
@@ -3692,7 +3696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A99">
         <v>2019</v>
       </c>
@@ -3717,7 +3721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A100">
         <v>2019</v>
       </c>
@@ -3742,7 +3746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A101">
         <v>2019</v>
       </c>
@@ -3767,7 +3771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A102">
         <v>2019</v>
       </c>
@@ -3792,7 +3796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A103">
         <v>2019</v>
       </c>
@@ -3817,7 +3821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A104">
         <v>2019</v>
       </c>
@@ -3842,7 +3846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A105">
         <v>2019</v>
       </c>
@@ -3867,7 +3871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A106">
         <v>2019</v>
       </c>
@@ -3902,7 +3906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A107">
         <v>2019</v>
       </c>
@@ -3939,7 +3943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A108">
         <v>2019</v>
       </c>
@@ -3976,7 +3980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A109">
         <v>2019</v>
       </c>
@@ -4013,7 +4017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A110">
         <v>2019</v>
       </c>
@@ -4050,7 +4054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A111">
         <v>2019</v>
       </c>
@@ -4087,7 +4091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A112">
         <v>2019</v>
       </c>
@@ -4124,7 +4128,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A113">
         <v>2019</v>
       </c>
@@ -4161,7 +4165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A114">
         <v>2019</v>
       </c>
@@ -4198,7 +4202,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A115">
         <v>2019</v>
       </c>
@@ -4235,7 +4239,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A116">
         <v>2019</v>
       </c>
@@ -4272,7 +4276,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A117">
         <v>2019</v>
       </c>
@@ -4309,7 +4313,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A118">
         <v>2019</v>
       </c>
@@ -4346,7 +4350,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A119">
         <v>2020</v>
       </c>
@@ -4383,7 +4387,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A120">
         <v>2020</v>
       </c>
@@ -4420,7 +4424,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A121">
         <v>2020</v>
       </c>
@@ -4457,7 +4461,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A122">
         <v>2020</v>
       </c>
@@ -4494,7 +4498,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A123">
         <v>2020</v>
       </c>
@@ -4531,7 +4535,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A124">
         <v>2020</v>
       </c>
@@ -4568,7 +4572,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A125">
         <v>2020</v>
       </c>
@@ -4605,7 +4609,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A126">
         <v>2020</v>
       </c>
@@ -4642,7 +4646,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A127">
         <v>2020</v>
       </c>
@@ -4679,7 +4683,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A128">
         <v>2020</v>
       </c>
@@ -4716,7 +4720,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A129">
         <v>2020</v>
       </c>
@@ -4753,7 +4757,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A130">
         <v>2020</v>
       </c>
@@ -4790,7 +4794,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A131">
         <v>2020</v>
       </c>
@@ -4827,7 +4831,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A132">
         <v>2020</v>
       </c>
@@ -4864,7 +4868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A133">
         <v>2020</v>
       </c>
@@ -4901,7 +4905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A134">
         <v>2020</v>
       </c>
@@ -4938,7 +4942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A135">
         <v>2020</v>
       </c>
@@ -4975,7 +4979,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A136">
         <v>2020</v>
       </c>
@@ -5012,7 +5016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A137">
         <v>2020</v>
       </c>
@@ -5049,7 +5053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A138">
         <v>2020</v>
       </c>
@@ -5086,7 +5090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A139">
         <v>2020</v>
       </c>
@@ -5111,7 +5115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A140">
         <v>2020</v>
       </c>
@@ -5136,7 +5140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A141">
         <v>2020</v>
       </c>
@@ -5161,7 +5165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A142">
         <v>2020</v>
       </c>
@@ -5186,7 +5190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A143">
         <v>2020</v>
       </c>
@@ -5211,7 +5215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A144">
         <v>2020</v>
       </c>
@@ -5236,7 +5240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A145">
         <v>2020</v>
       </c>
@@ -5261,7 +5265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A146">
         <v>2020</v>
       </c>
@@ -5286,7 +5290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A147">
         <v>2020</v>
       </c>
@@ -5311,7 +5315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A148">
         <v>2020</v>
       </c>
@@ -5336,7 +5340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A149">
         <v>2020</v>
       </c>
@@ -5361,7 +5365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A150">
         <v>2020</v>
       </c>
@@ -5386,7 +5390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A151">
         <v>2020</v>
       </c>
@@ -5411,7 +5415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A152">
         <v>2020</v>
       </c>
@@ -5436,7 +5440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A153">
         <v>2020</v>
       </c>
@@ -5461,7 +5465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A154">
         <v>2020</v>
       </c>
@@ -5486,7 +5490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A155">
         <v>2020</v>
       </c>
@@ -5511,7 +5515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A156">
         <v>2020</v>
       </c>
@@ -5536,7 +5540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A157">
         <v>2020</v>
       </c>
@@ -5561,7 +5565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A158">
         <v>2020</v>
       </c>
@@ -5569,7 +5573,7 @@
         <v>40</v>
       </c>
       <c r="C158" s="1">
-        <v>40448</v>
+        <v>44101</v>
       </c>
       <c r="D158" s="1">
         <v>44107</v>
@@ -5596,7 +5600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A159">
         <v>2020</v>
       </c>
@@ -5605,7 +5609,7 @@
       </c>
       <c r="C159" s="1">
         <f t="shared" ref="C159" si="35">C158+7</f>
-        <v>40455</v>
+        <v>44108</v>
       </c>
       <c r="D159" s="1">
         <f t="shared" ref="D159" si="36">D158+7</f>
@@ -5633,7 +5637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A160">
         <v>2020</v>
       </c>
@@ -5642,7 +5646,7 @@
       </c>
       <c r="C160" s="1">
         <f t="shared" ref="C160:C191" si="39">C159+7</f>
-        <v>40462</v>
+        <v>44115</v>
       </c>
       <c r="D160" s="1">
         <f t="shared" ref="D160:D191" si="40">D159+7</f>
@@ -5670,7 +5674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A161">
         <v>2020</v>
       </c>
@@ -5679,7 +5683,7 @@
       </c>
       <c r="C161" s="1">
         <f t="shared" si="39"/>
-        <v>40469</v>
+        <v>44122</v>
       </c>
       <c r="D161" s="1">
         <f t="shared" si="40"/>
@@ -5707,7 +5711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A162">
         <v>2020</v>
       </c>
@@ -5716,7 +5720,7 @@
       </c>
       <c r="C162" s="1">
         <f t="shared" si="39"/>
-        <v>40476</v>
+        <v>44129</v>
       </c>
       <c r="D162" s="1">
         <f t="shared" si="40"/>
@@ -5744,7 +5748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A163">
         <v>2020</v>
       </c>
@@ -5753,7 +5757,7 @@
       </c>
       <c r="C163" s="1">
         <f t="shared" si="39"/>
-        <v>40483</v>
+        <v>44136</v>
       </c>
       <c r="D163" s="1">
         <f t="shared" si="40"/>
@@ -5781,7 +5785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A164">
         <v>2020</v>
       </c>
@@ -5790,7 +5794,7 @@
       </c>
       <c r="C164" s="1">
         <f t="shared" si="39"/>
-        <v>40490</v>
+        <v>44143</v>
       </c>
       <c r="D164" s="1">
         <f t="shared" si="40"/>
@@ -5818,7 +5822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A165">
         <v>2020</v>
       </c>
@@ -5827,7 +5831,7 @@
       </c>
       <c r="C165" s="1">
         <f t="shared" si="39"/>
-        <v>40497</v>
+        <v>44150</v>
       </c>
       <c r="D165" s="1">
         <f t="shared" si="40"/>
@@ -5855,7 +5859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A166">
         <v>2020</v>
       </c>
@@ -5864,7 +5868,7 @@
       </c>
       <c r="C166" s="1">
         <f t="shared" si="39"/>
-        <v>40504</v>
+        <v>44157</v>
       </c>
       <c r="D166" s="1">
         <f t="shared" si="40"/>
@@ -5892,7 +5896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A167">
         <v>2020</v>
       </c>
@@ -5901,7 +5905,7 @@
       </c>
       <c r="C167" s="1">
         <f t="shared" si="39"/>
-        <v>40511</v>
+        <v>44164</v>
       </c>
       <c r="D167" s="1">
         <f t="shared" si="40"/>
@@ -5929,7 +5933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A168">
         <v>2020</v>
       </c>
@@ -5938,7 +5942,7 @@
       </c>
       <c r="C168" s="1">
         <f t="shared" si="39"/>
-        <v>40518</v>
+        <v>44171</v>
       </c>
       <c r="D168" s="1">
         <f t="shared" si="40"/>
@@ -5966,7 +5970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A169">
         <v>2020</v>
       </c>
@@ -5975,7 +5979,7 @@
       </c>
       <c r="C169" s="1">
         <f t="shared" si="39"/>
-        <v>40525</v>
+        <v>44178</v>
       </c>
       <c r="D169" s="1">
         <f t="shared" si="40"/>
@@ -6003,7 +6007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A170">
         <v>2020</v>
       </c>
@@ -6012,7 +6016,7 @@
       </c>
       <c r="C170" s="1">
         <f t="shared" si="39"/>
-        <v>40532</v>
+        <v>44185</v>
       </c>
       <c r="D170" s="1">
         <f t="shared" si="40"/>
@@ -6040,7 +6044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A171">
         <v>2020</v>
       </c>
@@ -6049,7 +6053,7 @@
       </c>
       <c r="C171" s="1">
         <f t="shared" si="39"/>
-        <v>40539</v>
+        <v>44192</v>
       </c>
       <c r="D171" s="1">
         <f t="shared" si="40"/>
@@ -6077,7 +6081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A172">
         <v>2021</v>
       </c>
@@ -6086,7 +6090,7 @@
       </c>
       <c r="C172" s="1">
         <f t="shared" si="39"/>
-        <v>40546</v>
+        <v>44199</v>
       </c>
       <c r="D172" s="1">
         <f t="shared" si="40"/>
@@ -6114,7 +6118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A173">
         <v>2021</v>
       </c>
@@ -6123,7 +6127,7 @@
       </c>
       <c r="C173" s="1">
         <f t="shared" si="39"/>
-        <v>40553</v>
+        <v>44206</v>
       </c>
       <c r="D173" s="1">
         <f t="shared" si="40"/>
@@ -6151,7 +6155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A174">
         <v>2021</v>
       </c>
@@ -6160,7 +6164,7 @@
       </c>
       <c r="C174" s="1">
         <f t="shared" si="39"/>
-        <v>40560</v>
+        <v>44213</v>
       </c>
       <c r="D174" s="1">
         <f t="shared" si="40"/>
@@ -6188,7 +6192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A175">
         <v>2021</v>
       </c>
@@ -6197,7 +6201,7 @@
       </c>
       <c r="C175" s="1">
         <f t="shared" si="39"/>
-        <v>40567</v>
+        <v>44220</v>
       </c>
       <c r="D175" s="1">
         <f t="shared" si="40"/>
@@ -6225,7 +6229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A176">
         <v>2021</v>
       </c>
@@ -6234,7 +6238,7 @@
       </c>
       <c r="C176" s="1">
         <f t="shared" si="39"/>
-        <v>40574</v>
+        <v>44227</v>
       </c>
       <c r="D176" s="1">
         <f t="shared" si="40"/>
@@ -6262,7 +6266,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A177">
         <v>2021</v>
       </c>
@@ -6271,7 +6275,7 @@
       </c>
       <c r="C177" s="1">
         <f t="shared" si="39"/>
-        <v>40581</v>
+        <v>44234</v>
       </c>
       <c r="D177" s="1">
         <f t="shared" si="40"/>
@@ -6299,7 +6303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A178">
         <v>2021</v>
       </c>
@@ -6308,7 +6312,7 @@
       </c>
       <c r="C178" s="1">
         <f t="shared" si="39"/>
-        <v>40588</v>
+        <v>44241</v>
       </c>
       <c r="D178" s="1">
         <f t="shared" si="40"/>
@@ -6336,7 +6340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A179">
         <v>2021</v>
       </c>
@@ -6345,7 +6349,7 @@
       </c>
       <c r="C179" s="1">
         <f t="shared" si="39"/>
-        <v>40595</v>
+        <v>44248</v>
       </c>
       <c r="D179" s="1">
         <f t="shared" si="40"/>
@@ -6373,7 +6377,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A180">
         <v>2021</v>
       </c>
@@ -6382,7 +6386,7 @@
       </c>
       <c r="C180" s="1">
         <f t="shared" si="39"/>
-        <v>40602</v>
+        <v>44255</v>
       </c>
       <c r="D180" s="1">
         <f t="shared" si="40"/>
@@ -6410,7 +6414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A181">
         <v>2021</v>
       </c>
@@ -6419,7 +6423,7 @@
       </c>
       <c r="C181" s="1">
         <f t="shared" si="39"/>
-        <v>40609</v>
+        <v>44262</v>
       </c>
       <c r="D181" s="1">
         <f t="shared" si="40"/>
@@ -6447,7 +6451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A182">
         <v>2021</v>
       </c>
@@ -6456,7 +6460,7 @@
       </c>
       <c r="C182" s="1">
         <f t="shared" si="39"/>
-        <v>40616</v>
+        <v>44269</v>
       </c>
       <c r="D182" s="1">
         <f t="shared" si="40"/>
@@ -6484,7 +6488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A183">
         <v>2021</v>
       </c>
@@ -6493,7 +6497,7 @@
       </c>
       <c r="C183" s="1">
         <f t="shared" si="39"/>
-        <v>40623</v>
+        <v>44276</v>
       </c>
       <c r="D183" s="1">
         <f t="shared" si="40"/>
@@ -6521,7 +6525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A184">
         <v>2021</v>
       </c>
@@ -6530,7 +6534,7 @@
       </c>
       <c r="C184" s="1">
         <f t="shared" si="39"/>
-        <v>40630</v>
+        <v>44283</v>
       </c>
       <c r="D184" s="1">
         <f t="shared" si="40"/>
@@ -6558,7 +6562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A185">
         <v>2021</v>
       </c>
@@ -6567,7 +6571,7 @@
       </c>
       <c r="C185" s="1">
         <f t="shared" si="39"/>
-        <v>40637</v>
+        <v>44290</v>
       </c>
       <c r="D185" s="1">
         <f t="shared" si="40"/>
@@ -6595,7 +6599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A186">
         <v>2021</v>
       </c>
@@ -6604,7 +6608,7 @@
       </c>
       <c r="C186" s="1">
         <f t="shared" si="39"/>
-        <v>40644</v>
+        <v>44297</v>
       </c>
       <c r="D186" s="1">
         <f t="shared" si="40"/>
@@ -6632,7 +6636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A187">
         <v>2021</v>
       </c>
@@ -6641,7 +6645,7 @@
       </c>
       <c r="C187" s="1">
         <f t="shared" si="39"/>
-        <v>40651</v>
+        <v>44304</v>
       </c>
       <c r="D187" s="1">
         <f t="shared" si="40"/>
@@ -6669,7 +6673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A188">
         <v>2021</v>
       </c>
@@ -6678,7 +6682,7 @@
       </c>
       <c r="C188" s="1">
         <f t="shared" si="39"/>
-        <v>40658</v>
+        <v>44311</v>
       </c>
       <c r="D188" s="1">
         <f t="shared" si="40"/>
@@ -6706,7 +6710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A189">
         <v>2021</v>
       </c>
@@ -6715,7 +6719,7 @@
       </c>
       <c r="C189" s="1">
         <f t="shared" si="39"/>
-        <v>40665</v>
+        <v>44318</v>
       </c>
       <c r="D189" s="1">
         <f t="shared" si="40"/>
@@ -6743,7 +6747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A190">
         <v>2021</v>
       </c>
@@ -6752,7 +6756,7 @@
       </c>
       <c r="C190" s="1">
         <f t="shared" si="39"/>
-        <v>40672</v>
+        <v>44325</v>
       </c>
       <c r="D190" s="1">
         <f t="shared" si="40"/>
@@ -6780,7 +6784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A191">
         <v>2021</v>
       </c>
@@ -6789,7 +6793,7 @@
       </c>
       <c r="C191" s="1">
         <f t="shared" si="39"/>
-        <v>40679</v>
+        <v>44332</v>
       </c>
       <c r="D191" s="1">
         <f t="shared" si="40"/>

</xml_diff>